<commit_message>
Se adicional un comentario en codigo y se corrige el archivo para git
</commit_message>
<xml_diff>
--- a/HU_TCS_AU.xlsx
+++ b/HU_TCS_AU.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Desktop\prueba choucair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A562AA59-5073-4201-A8A4-8243A133A839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F668D1D2-2D95-4C35-9A49-3A10212E1F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CBD3B9FC-ADD1-4D42-90ED-C3923FCCDD38}"/>
   </bookViews>
@@ -854,6 +854,51 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -872,33 +917,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -906,24 +924,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1242,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B457B36-EE05-426B-8441-DF42B4A84A58}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1270,28 +1270,28 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:4" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
@@ -1302,44 +1302,44 @@
       <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" spans="1:4" ht="78.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="145" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:4" ht="146.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:4" ht="164.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4" ht="220" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14" t="s">
@@ -1350,55 +1350,62 @@
       <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:4" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
     </row>
     <row r="15" spans="1:4" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
     </row>
     <row r="16" spans="1:4" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" ht="45.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A2:D2"/>
@@ -1408,13 +1415,6 @@
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>